<commit_message>
* added library dilution widget to dashboard * added sample receive feature in project page * added sequencer partition container deletion function for admins * added sample alias naming settings * added import and export sample library and pool sheet * added bulk 1d barcode printing
</commit_message>
<xml_diff>
--- a/core/src/main/resources/forms/ods/plate_input.xlsx
+++ b/core/src/main/resources/forms/ods/plate_input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23913"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="35000" yWindow="160" windowWidth="33600" windowHeight="19780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19320"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Paired</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Strategy</t>
   </si>
   <si>
-    <t>Illumina</t>
-  </si>
-  <si>
     <t>Plate position</t>
   </si>
   <si>
@@ -88,255 +85,6 @@
   </si>
   <si>
     <t>Converted pool molarity</t>
-  </si>
-  <si>
-    <t>LS454</t>
-  </si>
-  <si>
-    <t>PacBio</t>
-  </si>
-  <si>
-    <t>SOLiD</t>
-  </si>
-  <si>
-    <t>IonTorrent</t>
-  </si>
-  <si>
-    <t>Helicos</t>
-  </si>
-  <si>
-    <t>OTHER</t>
-  </si>
-  <si>
-    <t>RANDOM</t>
-  </si>
-  <si>
-    <t>PCR</t>
-  </si>
-  <si>
-    <t>RANDOM PCR</t>
-  </si>
-  <si>
-    <t>RT-PCR</t>
-  </si>
-  <si>
-    <t>HMPR</t>
-  </si>
-  <si>
-    <t>MF</t>
-  </si>
-  <si>
-    <t>CF-S</t>
-  </si>
-  <si>
-    <t>CF-M</t>
-  </si>
-  <si>
-    <t>CF-H</t>
-  </si>
-  <si>
-    <t>CF-T</t>
-  </si>
-  <si>
-    <t>MSLL</t>
-  </si>
-  <si>
-    <t>cDNA</t>
-  </si>
-  <si>
-    <t>ChIP</t>
-  </si>
-  <si>
-    <t>Mnase</t>
-  </si>
-  <si>
-    <t>DNAse</t>
-  </si>
-  <si>
-    <t>Hybrid Selection</t>
-  </si>
-  <si>
-    <t>Reduced Representation</t>
-  </si>
-  <si>
-    <t>Restriction Digest</t>
-  </si>
-  <si>
-    <t>5-methylcytidine antibody</t>
-  </si>
-  <si>
-    <t>MBD2 protein methyl-CpG binding domain</t>
-  </si>
-  <si>
-    <t>CAGE</t>
-  </si>
-  <si>
-    <t>RACE</t>
-  </si>
-  <si>
-    <t>size fractionation</t>
-  </si>
-  <si>
-    <t>MDA</t>
-  </si>
-  <si>
-    <t>padlock probes capture method</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>unspecified</t>
-  </si>
-  <si>
-    <t>WGS</t>
-  </si>
-  <si>
-    <t>WGA</t>
-  </si>
-  <si>
-    <t>WXS</t>
-  </si>
-  <si>
-    <t>RNA-Seq</t>
-  </si>
-  <si>
-    <t>WCS</t>
-  </si>
-  <si>
-    <t>MiRNA-Seq</t>
-  </si>
-  <si>
-    <t>CLONE</t>
-  </si>
-  <si>
-    <t>POOLCLONE</t>
-  </si>
-  <si>
-    <t>AMPLICON</t>
-  </si>
-  <si>
-    <t>CLONEEND</t>
-  </si>
-  <si>
-    <t>FINISHING</t>
-  </si>
-  <si>
-    <t>ChIP-Seq</t>
-  </si>
-  <si>
-    <t>Mnase-Seq</t>
-  </si>
-  <si>
-    <t>Dnase-Hypersensitivity</t>
-  </si>
-  <si>
-    <t>Bisulfite-Seq</t>
-  </si>
-  <si>
-    <t>EST</t>
-  </si>
-  <si>
-    <t>FL-cDNA</t>
-  </si>
-  <si>
-    <t>CTS</t>
-  </si>
-  <si>
-    <t>MRE-Seq</t>
-  </si>
-  <si>
-    <t>MeDIP-Seq</t>
-  </si>
-  <si>
-    <t>MBD-Seq</t>
-  </si>
-  <si>
-    <t>Tn-Seq</t>
-  </si>
-  <si>
-    <t>Platforms</t>
-  </si>
-  <si>
-    <t>Types</t>
-  </si>
-  <si>
-    <t>Selections</t>
-  </si>
-  <si>
-    <t>Strategies</t>
-  </si>
-  <si>
-    <t>Solid-Small RNA</t>
-  </si>
-  <si>
-    <t>Solid-Whole Transcriptome</t>
-  </si>
-  <si>
-    <t>Solid-SAGE</t>
-  </si>
-  <si>
-    <t>Solid-Long Mate Pair</t>
-  </si>
-  <si>
-    <t>Solid-Fragment</t>
-  </si>
-  <si>
-    <t>LS454-Amplicon</t>
-  </si>
-  <si>
-    <t>LS454-Transcriptome</t>
-  </si>
-  <si>
-    <t>LS454-20kbp Paired End</t>
-  </si>
-  <si>
-    <t>LS454-8kbp Paired End</t>
-  </si>
-  <si>
-    <t>LS454-3kbp Paired End</t>
-  </si>
-  <si>
-    <t>Illumina-mRNA Seq</t>
-  </si>
-  <si>
-    <t>Illumina-Mate Pair</t>
-  </si>
-  <si>
-    <t>Illumina-Paired End</t>
-  </si>
-  <si>
-    <t>Illumina-Small RNA</t>
-  </si>
-  <si>
-    <t>Illumina-Single End</t>
-  </si>
-  <si>
-    <t>LS454-Standard Shotgun</t>
-  </si>
-  <si>
-    <t>LS454-Rapid Shotgun</t>
-  </si>
-  <si>
-    <t>PacBio-10kb Shotgun</t>
-  </si>
-  <si>
-    <t>PacBio-20kb Shotgun</t>
-  </si>
-  <si>
-    <t>PacBio-2kb Shotgun</t>
-  </si>
-  <si>
-    <t>PacBio-Amplicon</t>
-  </si>
-  <si>
-    <t>PacBio-BAC</t>
-  </si>
-  <si>
-    <t>PacBio-Plasmid</t>
-  </si>
-  <si>
-    <t>PacBio-cDNA</t>
   </si>
   <si>
     <t>Pool Alias</t>
@@ -962,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:AC29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1017,24 +765,14 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="X1" s="4"/>
-      <c r="Y1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z1" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB1" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC1" s="17" t="s">
-        <v>81</v>
-      </c>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
       <c r="AMK1" s="4"/>
       <c r="AML1" s="4"/>
     </row>
@@ -1054,21 +792,10 @@
     </row>
     <row r="3" spans="1:32 1025:1026">
       <c r="X3" s="4"/>
-      <c r="Y3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC3" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="Z3" s="9"/>
+      <c r="AA3"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
       <c r="AE3"/>
       <c r="AF3"/>
       <c r="AMK3" s="4"/>
@@ -1076,90 +803,79 @@
     </row>
     <row r="4" spans="1:32 1025:1026">
       <c r="A4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="21" t="s">
+      <c r="D4" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="H4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="I4" s="21" t="s">
+      <c r="J4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="K4" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="L4" s="21" t="s">
+      <c r="M4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="N4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="O4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="P4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="Q4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="R4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="S4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="T4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="V4" s="21" t="s">
+      <c r="W4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="W4" s="21" t="s">
-        <v>22</v>
-      </c>
       <c r="X4" s="4"/>
-      <c r="Y4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>93</v>
-      </c>
-      <c r="AB4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC4" s="9" t="s">
-        <v>57</v>
-      </c>
+      <c r="Z4" s="9"/>
+      <c r="AA4"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
       <c r="AE4"/>
       <c r="AF4"/>
       <c r="AMK4" s="4"/>
@@ -1180,18 +896,10 @@
       <c r="R5" s="13"/>
       <c r="U5" s="13"/>
       <c r="X5" s="4"/>
-      <c r="Z5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC5" s="9" t="s">
-        <v>58</v>
-      </c>
+      <c r="Z5" s="9"/>
+      <c r="AA5"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
       <c r="AE5"/>
       <c r="AF5"/>
       <c r="AMK5" s="4"/>
@@ -1213,18 +921,10 @@
       <c r="S6" s="13"/>
       <c r="U6" s="13"/>
       <c r="X6" s="4"/>
-      <c r="Z6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC6" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="Z6" s="9"/>
+      <c r="AA6"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
       <c r="AE6"/>
       <c r="AF6"/>
       <c r="AMK6" s="4"/>
@@ -1244,18 +944,10 @@
       <c r="Q7" s="13"/>
       <c r="U7" s="13"/>
       <c r="X7" s="4"/>
-      <c r="Z7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC7" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="Z7" s="9"/>
+      <c r="AA7"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
       <c r="AE7"/>
       <c r="AF7"/>
       <c r="AMK7" s="4"/>
@@ -1275,18 +967,10 @@
       <c r="Q8" s="13"/>
       <c r="U8" s="13"/>
       <c r="X8" s="4"/>
-      <c r="Z8" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB8" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC8" s="9" t="s">
-        <v>61</v>
-      </c>
+      <c r="Z8" s="9"/>
+      <c r="AA8"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
       <c r="AE8"/>
       <c r="AF8"/>
       <c r="AMK8" s="4"/>
@@ -1307,15 +991,9 @@
       <c r="U9" s="13"/>
       <c r="X9" s="4"/>
       <c r="Z9" s="15"/>
-      <c r="AA9" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC9" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="AA9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
       <c r="AE9"/>
       <c r="AF9"/>
       <c r="AMK9" s="4"/>
@@ -1336,15 +1014,9 @@
       <c r="U10" s="13"/>
       <c r="X10" s="4"/>
       <c r="Z10" s="5"/>
-      <c r="AA10" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC10" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="AA10"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
       <c r="AE10"/>
       <c r="AF10"/>
       <c r="AMK10" s="4"/>
@@ -1365,15 +1037,9 @@
       <c r="U11" s="13"/>
       <c r="X11" s="4"/>
       <c r="Z11" s="9"/>
-      <c r="AA11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB11" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC11" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="AA11"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
       <c r="AE11"/>
       <c r="AF11"/>
       <c r="AMK11" s="4"/>
@@ -1394,15 +1060,9 @@
       <c r="U12" s="13"/>
       <c r="X12" s="4"/>
       <c r="Z12" s="9"/>
-      <c r="AA12" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB12" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC12" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="AA12"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
       <c r="AE12"/>
       <c r="AF12"/>
       <c r="AMK12" s="4"/>
@@ -1423,15 +1083,9 @@
       <c r="U13" s="13"/>
       <c r="X13" s="4"/>
       <c r="Z13" s="9"/>
-      <c r="AA13" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB13" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC13" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="AA13"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
       <c r="AE13"/>
       <c r="AF13"/>
       <c r="AMK13" s="4"/>
@@ -1454,15 +1108,9 @@
       <c r="U14" s="13"/>
       <c r="X14" s="4"/>
       <c r="Z14" s="9"/>
-      <c r="AA14" t="s">
-        <v>98</v>
-      </c>
-      <c r="AB14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC14" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="AA14"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
       <c r="AE14"/>
       <c r="AF14"/>
       <c r="AMK14" s="4"/>
@@ -1482,15 +1130,9 @@
       <c r="Q15" s="13"/>
       <c r="X15" s="4"/>
       <c r="Z15" s="9"/>
-      <c r="AA15" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB15" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC15" s="9" t="s">
-        <v>68</v>
-      </c>
+      <c r="AA15"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
       <c r="AE15"/>
       <c r="AF15"/>
       <c r="AMK15" s="4"/>
@@ -1510,15 +1152,9 @@
       <c r="Q16" s="13"/>
       <c r="X16" s="4"/>
       <c r="Z16" s="9"/>
-      <c r="AA16" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC16" s="9" t="s">
-        <v>69</v>
-      </c>
+      <c r="AA16"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
       <c r="AE16"/>
       <c r="AF16"/>
       <c r="AMK16" s="4"/>
@@ -1538,15 +1174,9 @@
       <c r="Q17" s="13"/>
       <c r="X17" s="4"/>
       <c r="Z17" s="9"/>
-      <c r="AA17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB17" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC17" s="9" t="s">
-        <v>70</v>
-      </c>
+      <c r="AA17"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
       <c r="AE17"/>
       <c r="AF17"/>
       <c r="AMK17" s="4"/>
@@ -1566,15 +1196,9 @@
       <c r="Q18" s="13"/>
       <c r="X18" s="4"/>
       <c r="Z18" s="9"/>
-      <c r="AA18" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB18" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC18" s="9" t="s">
-        <v>71</v>
-      </c>
+      <c r="AA18"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
       <c r="AE18"/>
       <c r="AF18"/>
       <c r="AMK18" s="4"/>
@@ -1594,15 +1218,9 @@
       <c r="Q19" s="13"/>
       <c r="X19" s="4"/>
       <c r="Z19" s="15"/>
-      <c r="AA19" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB19" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC19" s="9" t="s">
-        <v>72</v>
-      </c>
+      <c r="AA19"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
       <c r="AE19"/>
       <c r="AF19"/>
       <c r="AMK19" s="4"/>
@@ -1622,15 +1240,9 @@
       <c r="Q20" s="13"/>
       <c r="X20" s="4"/>
       <c r="Z20" s="15"/>
-      <c r="AA20" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB20" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC20" s="9" t="s">
-        <v>73</v>
-      </c>
+      <c r="AA20"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="9"/>
       <c r="AMK20" s="4"/>
       <c r="AML20" s="4"/>
     </row>
@@ -1648,87 +1260,53 @@
       <c r="Q21" s="13"/>
       <c r="X21" s="4"/>
       <c r="Z21" s="15"/>
-      <c r="AA21" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB21" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC21" s="9" t="s">
-        <v>74</v>
-      </c>
+      <c r="AA21"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
       <c r="AMK21" s="4"/>
       <c r="AML21" s="4"/>
     </row>
     <row r="22" spans="5:32 1025:1026">
       <c r="X22" s="4"/>
       <c r="Z22" s="15"/>
-      <c r="AA22" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB22" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC22" s="9" t="s">
-        <v>75</v>
-      </c>
+      <c r="AA22"/>
+      <c r="AB22" s="9"/>
+      <c r="AC22" s="9"/>
       <c r="AMK22" s="4"/>
       <c r="AML22" s="4"/>
     </row>
     <row r="23" spans="5:32 1025:1026">
       <c r="X23" s="4"/>
       <c r="Z23" s="15"/>
-      <c r="AA23" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB23" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC23" s="9" t="s">
-        <v>76</v>
-      </c>
+      <c r="AA23"/>
+      <c r="AB23" s="9"/>
+      <c r="AC23" s="9"/>
       <c r="AMK23" s="4"/>
       <c r="AML23" s="4"/>
     </row>
     <row r="24" spans="5:32 1025:1026">
       <c r="X24" s="4"/>
       <c r="Z24" s="15"/>
-      <c r="AA24" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB24" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC24" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="AA24"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="9"/>
       <c r="AMK24" s="4"/>
       <c r="AML24" s="4"/>
     </row>
     <row r="25" spans="5:32 1025:1026">
       <c r="X25" s="4"/>
       <c r="Z25" s="15"/>
-      <c r="AA25" t="s">
-        <v>104</v>
-      </c>
-      <c r="AB25" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC25" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="AA25"/>
+      <c r="AB25" s="9"/>
+      <c r="AC25" s="9"/>
       <c r="AMK25" s="4"/>
       <c r="AML25" s="4"/>
     </row>
     <row r="26" spans="5:32 1025:1026">
       <c r="X26" s="4"/>
       <c r="Z26" s="15"/>
-      <c r="AA26" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB26" s="9" t="s">
-        <v>52</v>
-      </c>
+      <c r="AA26"/>
+      <c r="AB26" s="9"/>
       <c r="AMK26" s="4"/>
       <c r="AML26" s="4"/>
     </row>
@@ -1736,9 +1314,7 @@
       <c r="X27" s="4"/>
       <c r="Z27" s="15"/>
       <c r="AA27"/>
-      <c r="AB27" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="AB27" s="9"/>
       <c r="AMK27" s="4"/>
       <c r="AML27" s="4"/>
     </row>
@@ -1746,9 +1322,7 @@
       <c r="X28" s="4"/>
       <c r="Z28" s="15"/>
       <c r="AA28"/>
-      <c r="AB28" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="AB28" s="9"/>
       <c r="AMK28" s="4"/>
       <c r="AML28" s="4"/>
     </row>
@@ -1756,9 +1330,7 @@
       <c r="X29" s="4"/>
       <c r="Z29" s="15"/>
       <c r="AA29"/>
-      <c r="AB29" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="AB29" s="9"/>
       <c r="AMK29" s="4"/>
       <c r="AML29" s="4"/>
     </row>

</xml_diff>